<commit_message>
Testes com a base de dados no Excel
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filipe.nascimento\Desktop\autoVinculo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B97565-6AF3-4155-BBAA-98A5B3AEFD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9139A60F-E51B-42C0-9A5E-553C897FA2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{642F9480-EF3D-4509-A38C-60246068E5DF}"/>
   </bookViews>
@@ -34,20 +34,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>nomeVendedor</t>
   </si>
   <si>
-    <t>Michele</t>
-  </si>
-  <si>
     <t>cnpj</t>
   </si>
   <si>
-    <t>qntVinculos</t>
-  </si>
-  <si>
     <t>tipoTabela</t>
   </si>
   <si>
@@ -57,37 +51,25 @@
     <t>Origem</t>
   </si>
   <si>
-    <t>SAO</t>
-  </si>
-  <si>
     <t>seTaxa</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>tipoTaxa</t>
   </si>
   <si>
     <t>taxa</t>
   </si>
   <si>
-    <t>PACKAGE</t>
-  </si>
-  <si>
-    <t>0.75</t>
-  </si>
-  <si>
     <t>.COM 2</t>
   </si>
   <si>
-    <t>.COM</t>
-  </si>
-  <si>
-    <t>Pickup</t>
-  </si>
-  <si>
-    <t>PICKUP</t>
+    <t>Erik</t>
+  </si>
+  <si>
+    <t>SSA</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -123,9 +105,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -442,126 +427,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C9F820-D428-4127-9068-B7A471FB8600}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>20400219000195</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>20400219000195</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>43025888000120</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>43025888000120</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>43025888000120</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>13</v>
-      </c>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correções de Bugs e Estruturas do Banco de Dados.
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filipe.nascimento\Desktop\autoVinculo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5067EC-3D43-40D8-8B53-45B857F4270B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E2266C-B7E3-484F-8BDD-5EC501DA9FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{642F9480-EF3D-4509-A38C-60246068E5DF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>nomeVendedor</t>
   </si>
@@ -45,9 +45,6 @@
     <t>tipoTabela</t>
   </si>
   <si>
-    <t>Package 4</t>
-  </si>
-  <si>
     <t>Origem</t>
   </si>
   <si>
@@ -60,13 +57,19 @@
     <t>taxa</t>
   </si>
   <si>
-    <t>Erik</t>
-  </si>
-  <si>
-    <t>SSA</t>
-  </si>
-  <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Naiara</t>
+  </si>
+  <si>
+    <t>SAO</t>
+  </si>
+  <si>
+    <t>Package 2</t>
+  </si>
+  <si>
+    <t>.COM 2</t>
   </si>
 </sst>
 </file>
@@ -102,13 +105,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -424,21 +433,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C9F820-D428-4127-9068-B7A471FB8600}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="1" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,33 +457,33 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1">
-        <v>20400219000195</v>
+      <c r="B2" s="3">
+        <v>30466928000127</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -484,16 +492,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3">
+        <v>30466928000127</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -502,6 +524,9 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J11" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Melhorias no scriptVync e Mudanças no scriptEmail.
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filipe.nascimento\Desktop\autoVinculo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E2266C-B7E3-484F-8BDD-5EC501DA9FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A50209E-AF93-4B3A-8030-EB7423B51305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{642F9480-EF3D-4509-A38C-60246068E5DF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>nomeVendedor</t>
   </si>
@@ -70,6 +70,30 @@
   </si>
   <si>
     <t>.COM 2</t>
+  </si>
+  <si>
+    <t>Michele</t>
+  </si>
+  <si>
+    <t>12424533476839</t>
+  </si>
+  <si>
+    <t>Pickup</t>
+  </si>
+  <si>
+    <t>RIO</t>
+  </si>
+  <si>
+    <t>Erik</t>
+  </si>
+  <si>
+    <t>Package 1</t>
+  </si>
+  <si>
+    <t>BHZ</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -436,7 +460,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,13 +540,50 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3">
+        <v>52346238428828</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J11" s="4"/>

</xml_diff>

<commit_message>
Adicionando função de email com CNPJ duplicado.
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filipe.nascimento\Desktop\autoVinculo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6280EFDB-261D-4E6C-91D4-C5D0CDC56552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EEFB89-B371-4DA6-82B8-ACE47D278A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{642F9480-EF3D-4509-A38C-60246068E5DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
-    <sheet name="Dezembro" sheetId="3" state="hidden" r:id="rId2"/>
-    <sheet name="Configurações" sheetId="2" r:id="rId3"/>
+    <sheet name="Dezembro" sheetId="3" r:id="rId2"/>
+    <sheet name="Configurações" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="101">
   <si>
     <t>nomeVendedor</t>
   </si>
@@ -337,6 +337,9 @@
   <si>
     <t>Não</t>
   </si>
+  <si>
+    <t>Package 1</t>
+  </si>
 </sst>
 </file>
 
@@ -418,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -446,6 +449,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1206,7 +1213,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,10 +1252,10 @@
         <v>97</v>
       </c>
       <c r="B2" s="4">
-        <v>39918899000161</v>
+        <v>43101014000104</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>26</v>
@@ -1260,7 +1267,7 @@
         <v>87</v>
       </c>
       <c r="G2" s="3">
-        <v>2.95</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1268,7 +1275,7 @@
         <v>97</v>
       </c>
       <c r="B3" s="4">
-        <v>39918899000161</v>
+        <v>43101014000104</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>14</v>
@@ -1283,7 +1290,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="3">
-        <v>2.95</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1294,6 +1301,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
+      <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -10298,18 +10306,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EC228D-6414-49BA-B283-950DCE95B980}">
-  <dimension ref="A2:P16"/>
+  <dimension ref="A2:S18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="7" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="7" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="14" width="9.140625" style="7" customWidth="1"/>
@@ -10355,48 +10363,94 @@
       </c>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="13">
+        <v>39918899000161</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I15" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="13">
+        <v>39918899000161</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D17" s="13">
         <v>42653898000147</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G17" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H17" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I17" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C16" s="9" t="s">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D18" s="13">
         <v>42653898000147</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G18" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I18" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -10410,25 +10464,25 @@
           <x14:formula1>
             <xm:f>Configurações!$H$3:$H$12</xm:f>
           </x14:formula1>
-          <xm:sqref>H15:H16</xm:sqref>
+          <xm:sqref>H15:H18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ED7221E5-90E5-4E57-953C-2EBE44490DC4}">
           <x14:formula1>
             <xm:f>Configurações!$F$3:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G15:G16</xm:sqref>
+          <xm:sqref>G15:G18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5DBF407A-E5B5-4ADB-A42B-762DE44E1343}">
           <x14:formula1>
             <xm:f>Configurações!$B$3:$B$71</xm:f>
           </x14:formula1>
-          <xm:sqref>F15:F16</xm:sqref>
+          <xm:sqref>F15:F18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F3C01477-BD71-4418-BF61-26DC577C567E}">
           <x14:formula1>
             <xm:f>Configurações!$D$3:$D$14</xm:f>
           </x14:formula1>
-          <xm:sqref>E15:E16</xm:sqref>
+          <xm:sqref>E15:E18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Atualizando listagem d/Taxa, Melhorias ScriptEmail
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filipe.nascimento\Desktop\autoVinculo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filipe.nascimento\Desktop\vync\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EEFB89-B371-4DA6-82B8-ACE47D278A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F25676-6F89-4837-87D0-39C793A2A608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{642F9480-EF3D-4509-A38C-60246068E5DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
-    <sheet name="Dezembro" sheetId="3" r:id="rId2"/>
+    <sheet name="Dezembro.2021" sheetId="3" r:id="rId2"/>
     <sheet name="Configurações" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="103">
   <si>
     <t>nomeVendedor</t>
   </si>
@@ -323,12 +323,6 @@
     <t>EMERGENCIAL</t>
   </si>
   <si>
-    <t>Última atualização: 06/10/2021</t>
-  </si>
-  <si>
-    <t>*Faz a importação da base de dados</t>
-  </si>
-  <si>
     <t>Naiara</t>
   </si>
   <si>
@@ -339,6 +333,18 @@
   </si>
   <si>
     <t>Package 1</t>
+  </si>
+  <si>
+    <t>Maristela</t>
+  </si>
+  <si>
+    <t>Vendedores</t>
+  </si>
+  <si>
+    <t>Michele</t>
+  </si>
+  <si>
+    <t>Thiago</t>
   </si>
 </sst>
 </file>
@@ -472,80 +478,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1085850</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Retângulo: Cantos Arredondados 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B880B9EA-32C0-40D8-BFC5-0B0EC3368706}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="600075" y="1714500"/>
-          <a:ext cx="2114550" cy="542925"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="C00000"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1400"/>
-            <a:t>Importar</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1400" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:endParaRPr lang="pt-BR" sz="1400"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -691,187 +623,73 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>361949</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>380999</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="CaixaDeTexto 7">
+        <xdr:cNvPr id="4" name="Retângulo: Cantos Arredondados 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72AE4139-7E05-4576-BB43-A3FC59247F9F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B880B9EA-32C0-40D8-BFC5-0B0EC3368706}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="552449" y="1123950"/>
-          <a:ext cx="4333875" cy="371475"/>
+          <a:off x="9686925" y="857250"/>
+          <a:ext cx="2038350" cy="542925"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom prst="roundRect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
+        <a:solidFill>
+          <a:srgbClr val="C00000"/>
+        </a:solidFill>
+        <a:ln>
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
         </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="pt-BR" sz="1800">
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Cadastros</a:t>
+            <a:rPr lang="pt-BR" sz="1400"/>
+            <a:t>Importar</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="pt-BR" sz="1800" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> Realizados/Relatório de Cadastros</a:t>
-          </a:r>
-          <a:endParaRPr lang="pt-BR" sz="1800">
-            <a:solidFill>
-              <a:srgbClr val="C00000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="CaixaDeTexto 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2EBC69E-A9BD-4D6E-8888-08AE4203D770}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9515475" y="657225"/>
-          <a:ext cx="2686050" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Obs:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR"/>
+            <a:rPr lang="pt-BR" sz="1400" baseline="0"/>
             <a:t> </a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Sempre</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> renomear as abas com o mês. </a:t>
-          </a:r>
-          <a:endParaRPr lang="pt-BR" sz="1100"/>
+          <a:endParaRPr lang="pt-BR" sz="1400"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1213,7 +1031,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,6 +1040,7 @@
     <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1249,122 +1068,206 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4">
-        <v>43101014000104</v>
+        <v>14067302000191</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>87</v>
       </c>
       <c r="G2" s="3">
-        <v>1.95</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" s="4">
-        <v>43101014000104</v>
+        <v>37031122000155</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="4">
+        <v>18327363000100</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2.95</v>
+      </c>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="4">
+        <v>18327363000100</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3">
-        <v>1.95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="14"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="G5" s="3">
+        <v>2.95</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="A6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="4">
+        <v>18327363000100</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="5"/>
+      <c r="A7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="4">
+        <v>18327363000100</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2.95</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="5"/>
+      <c r="A8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="4">
+        <v>18327363000100</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2.95</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="5"/>
+      <c r="A9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="4">
+        <v>18327363000100</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="3">
+        <v>2.95</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="5"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="5"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="5"/>
+      <c r="G11" s="3"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -10276,7 +10179,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F3C01477-BD71-4418-BF61-26DC577C567E}">
           <x14:formula1>
-            <xm:f>Configurações!$D$3:$D$14</xm:f>
+            <xm:f>Configurações!$D$3:$D$17</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1000</xm:sqref>
         </x14:dataValidation>
@@ -10306,10 +10209,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EC228D-6414-49BA-B283-950DCE95B980}">
-  <dimension ref="A2:S18"/>
+  <dimension ref="A2:S20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10329,160 +10232,258 @@
     <row r="2" spans="3:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="3:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="P6" s="12" t="s">
+      <c r="P6" s="12"/>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C8" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="11" spans="3:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D9" s="4">
+        <v>43101014000104</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="4">
+        <v>43101014000104</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="13">
+        <v>39918899000161</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="13">
+        <v>39918899000161</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="H12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="13">
+        <v>42653898000147</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C14" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>6</v>
+      <c r="C14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="13">
+        <v>42653898000147</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D15" s="13">
-        <v>39918899000161</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I15" s="3">
-        <v>2.95</v>
-      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="13">
-        <v>39918899000161</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="3">
-        <v>2.95</v>
-      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="13">
-        <v>42653898000147</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>10</v>
-      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="13">
-        <v>42653898000147</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>10</v>
-      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="2"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="2"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0F8627C6-C092-4293-9362-50A35151177D}">
           <x14:formula1>
             <xm:f>Configurações!$H$3:$H$12</xm:f>
           </x14:formula1>
-          <xm:sqref>H15:H18</xm:sqref>
+          <xm:sqref>H9:H14 H17:H20 H15:H16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ED7221E5-90E5-4E57-953C-2EBE44490DC4}">
           <x14:formula1>
             <xm:f>Configurações!$F$3:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G15:G18</xm:sqref>
+          <xm:sqref>G9:G14 G17:G20 G15:G16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5DBF407A-E5B5-4ADB-A42B-762DE44E1343}">
           <x14:formula1>
             <xm:f>Configurações!$B$3:$B$71</xm:f>
           </x14:formula1>
-          <xm:sqref>F15:F18</xm:sqref>
+          <xm:sqref>F9:F14 F17:F20 F15:F16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F3C01477-BD71-4418-BF61-26DC577C567E}">
           <x14:formula1>
             <xm:f>Configurações!$D$3:$D$14</xm:f>
           </x14:formula1>
-          <xm:sqref>E15:E18</xm:sqref>
+          <xm:sqref>E9:E14</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5FFB896A-E7BF-415F-B2C3-F7420D88CEEF}">
+          <x14:formula1>
+            <xm:f>Configurações!$D$3:$D$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>E17:E20 E15:E16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10492,10 +10493,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0422754E-9E82-42E9-B445-88A740DA2705}">
-  <dimension ref="B2:H71"/>
+  <dimension ref="B2:J71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10508,10 +10509,12 @@
     <col min="6" max="6" width="9.140625" style="7"/>
     <col min="7" max="7" width="3.140625" style="7" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="7"/>
+    <col min="9" max="9" width="3.7109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
@@ -10524,8 +10527,11 @@
       <c r="H2" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J2" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>86</v>
       </c>
@@ -10533,13 +10539,16 @@
         <v>16</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>26</v>
       </c>
@@ -10547,13 +10556,16 @@
         <v>13</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>27</v>
       </c>
@@ -10563,8 +10575,11 @@
       <c r="H5" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J5" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>28</v>
       </c>
@@ -10574,8 +10589,11 @@
       <c r="H6" s="8" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J6" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>29</v>
       </c>
@@ -10585,8 +10603,11 @@
       <c r="H7" s="8" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>30</v>
       </c>
@@ -10596,8 +10617,9 @@
       <c r="H8" s="8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
@@ -10607,8 +10629,9 @@
       <c r="H9" s="8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>31</v>
       </c>
@@ -10618,8 +10641,9 @@
       <c r="H10" s="8" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>32</v>
       </c>
@@ -10629,8 +10653,9 @@
       <c r="H11" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>33</v>
       </c>
@@ -10640,8 +10665,9 @@
       <c r="H12" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>34</v>
       </c>
@@ -10649,7 +10675,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>35</v>
       </c>
@@ -10657,92 +10683,101 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D16" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D17" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Testes, Melhorias no scriptVync.
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filipe.nascimento\Desktop\vync\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F25676-6F89-4837-87D0-39C793A2A608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236B9161-FA87-4AF0-975C-13ACA672A67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{642F9480-EF3D-4509-A38C-60246068E5DF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="103">
   <si>
     <t>nomeVendedor</t>
   </si>
@@ -1031,7 +1031,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,188 +1068,86 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="B2" s="4">
-        <v>14067302000191</v>
+        <v>43101014000104</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" s="3">
-        <v>2.95</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="4">
-        <v>37031122000155</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" s="3">
-        <v>4.5</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="4">
-        <v>18327363000100</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G4" s="3">
-        <v>2.95</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="4">
-        <v>18327363000100</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="3">
-        <v>2.95</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="4">
-        <v>18327363000100</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="4">
-        <v>18327363000100</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G7" s="3">
-        <v>2.95</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="4">
-        <v>18327363000100</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G8" s="3">
-        <v>2.95</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B9" s="4">
-        <v>18327363000100</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G9" s="3">
-        <v>2.95</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -10176,12 +10074,12 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F3C01477-BD71-4418-BF61-26DC577C567E}">
           <x14:formula1>
             <xm:f>Configurações!$D$3:$D$17</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1000</xm:sqref>
+          <xm:sqref>C3:C1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5DBF407A-E5B5-4ADB-A42B-762DE44E1343}">
           <x14:formula1>
@@ -10201,6 +10099,12 @@
           </x14:formula1>
           <xm:sqref>F2:F1000</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{385F2494-8E49-4EB2-B697-468D7EDEBD4E}">
+          <x14:formula1>
+            <xm:f>Configurações!$D$3:$D$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -10209,10 +10113,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EC228D-6414-49BA-B283-950DCE95B980}">
-  <dimension ref="A2:S20"/>
+  <dimension ref="A2:S30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10396,58 +10300,356 @@
       </c>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="2"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="4">
+        <v>14067302000191</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I15" s="3">
+        <v>2.95</v>
+      </c>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C16" s="2"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="C16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="4">
+        <v>37031122000155</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I16" s="3">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="2"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="C17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="4">
+        <v>18327363000100</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" s="3">
+        <v>2.95</v>
+      </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="2"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="C18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="4">
+        <v>18327363000100</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="3">
+        <v>2.95</v>
+      </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="2"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="C19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="4">
+        <v>18327363000100</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="2"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="C20" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="4">
+        <v>18327363000100</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="4">
+        <v>18327363000100</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I21" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="4">
+        <v>18327363000100</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="4">
+        <v>30305913000187</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="4">
+        <v>30305913000187</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="4">
+        <v>33882082000102</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="4">
+        <v>33882082000102</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="4">
+        <v>31462702000110</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="4">
+        <v>31462702000110</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="4">
+        <v>32110318000111</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="4">
+        <v>32110318000111</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="3">
+        <v>1.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -10459,19 +10661,19 @@
           <x14:formula1>
             <xm:f>Configurações!$H$3:$H$12</xm:f>
           </x14:formula1>
-          <xm:sqref>H9:H14 H17:H20 H15:H16</xm:sqref>
+          <xm:sqref>H9:H30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ED7221E5-90E5-4E57-953C-2EBE44490DC4}">
           <x14:formula1>
             <xm:f>Configurações!$F$3:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G9:G14 G17:G20 G15:G16</xm:sqref>
+          <xm:sqref>G9:G30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5DBF407A-E5B5-4ADB-A42B-762DE44E1343}">
           <x14:formula1>
             <xm:f>Configurações!$B$3:$B$71</xm:f>
           </x14:formula1>
-          <xm:sqref>F9:F14 F17:F20 F15:F16</xm:sqref>
+          <xm:sqref>F9:F30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F3C01477-BD71-4418-BF61-26DC577C567E}">
           <x14:formula1>
@@ -10479,11 +10681,11 @@
           </x14:formula1>
           <xm:sqref>E9:E14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5FFB896A-E7BF-415F-B2C3-F7420D88CEEF}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A233C3B7-4BB9-4561-A5A2-008CD85E80B5}">
           <x14:formula1>
             <xm:f>Configurações!$D$3:$D$17</xm:f>
           </x14:formula1>
-          <xm:sqref>E17:E20 E15:E16</xm:sqref>
+          <xm:sqref>E15:E30</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Adicionando MultiOrigem no DF.
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filipe.nascimento\Desktop\vync\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD90AEF2-A585-4A87-A1F1-657462D0C26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F8D4A0-BAB0-4812-8350-2F9626E32757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{642F9480-EF3D-4509-A38C-60246068E5DF}"/>
   </bookViews>
@@ -486,86 +486,18 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Retângulo 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02EB3986-EBB4-4DCD-9F58-CC6E5FC649C9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="619125" y="371475"/>
-          <a:ext cx="12163425" cy="809625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1">
-            <a:lumMod val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="pt-BR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>500488</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>367138</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -619,7 +551,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="276225" y="323850"/>
+          <a:off x="142875" y="0"/>
           <a:ext cx="1853038" cy="923925"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -627,80 +559,6 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Retângulo: Cantos Arredondados 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B880B9EA-32C0-40D8-BFC5-0B0EC3368706}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9686925" y="857250"/>
-          <a:ext cx="2038350" cy="542925"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="C00000"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1400"/>
-            <a:t>Importar</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1400" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:endParaRPr lang="pt-BR" sz="1400"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -10105,10 +9963,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EC228D-6414-49BA-B283-950DCE95B980}">
-  <dimension ref="A2:S59"/>
+  <dimension ref="A2:S56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K58" sqref="K58"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10127,41 +9985,108 @@
   <sheetData>
     <row r="2" spans="3:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="3:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="4">
+        <v>43101014000104</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1.95</v>
+      </c>
       <c r="P6" s="11"/>
     </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="4">
+        <v>43101014000104</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1.95</v>
+      </c>
+    </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>6</v>
+      <c r="C8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="12">
+        <v>39918899000161</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8" s="3">
+        <v>2.95</v>
       </c>
     </row>
     <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="4">
-        <v>43101014000104</v>
+      <c r="D9" s="12">
+        <v>39918899000161</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>98</v>
+        <v>14</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>26</v>
@@ -10170,145 +10095,145 @@
         <v>96</v>
       </c>
       <c r="H9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="12">
+        <v>42653898000147</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="I9" s="3">
-        <v>1.95</v>
-      </c>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="4">
-        <v>43101014000104</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="12">
+        <v>42653898000147</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="3">
-        <v>1.95</v>
-      </c>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="12">
-        <v>39918899000161</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I11" s="3">
-        <v>2.95</v>
+      <c r="I11" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="12">
-        <v>39918899000161</v>
+        <v>7</v>
+      </c>
+      <c r="D12" s="4">
+        <v>14067302000191</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>96</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="I12" s="3">
         <v>2.95</v>
       </c>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="12">
-        <v>42653898000147</v>
-      </c>
-      <c r="E13" s="8" t="s">
+      <c r="C13" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="4">
+        <v>37031122000155</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I13" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="4">
+        <v>18327363000100</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="9" t="s">
+      <c r="F14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="I13" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="12">
-        <v>42653898000147</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>10</v>
+      <c r="I14" s="3">
+        <v>2.95</v>
       </c>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="D15" s="4">
-        <v>14067302000191</v>
+        <v>18327363000100</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>96</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="I15" s="3">
         <v>2.95</v>
@@ -10319,10 +10244,10 @@
         <v>95</v>
       </c>
       <c r="D16" s="4">
-        <v>37031122000155</v>
+        <v>18327363000100</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>26</v>
@@ -10331,10 +10256,10 @@
         <v>96</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="I16" s="3">
-        <v>4.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
@@ -10345,7 +10270,7 @@
         <v>18327363000100</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>26</v>
@@ -10354,7 +10279,7 @@
         <v>96</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="I17" s="3">
         <v>2.95</v>
@@ -10368,7 +10293,7 @@
         <v>18327363000100</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>26</v>
@@ -10377,7 +10302,7 @@
         <v>96</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="I18" s="3">
         <v>2.95</v>
@@ -10391,7 +10316,7 @@
         <v>18327363000100</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>26</v>
@@ -10400,90 +10325,78 @@
         <v>96</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="I19" s="3">
-        <v>1</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="D20" s="4">
-        <v>18327363000100</v>
+        <v>30305913000187</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I20" s="3">
-        <v>2.95</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="D21" s="4">
-        <v>18327363000100</v>
+        <v>30305913000187</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="I21" s="3">
-        <v>2.95</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="D22" s="4">
-        <v>18327363000100</v>
+        <v>33882082000102</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="I22" s="3">
-        <v>2.95</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="4">
-        <v>30305913000187</v>
+        <v>33882082000102</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>8</v>
@@ -10496,184 +10409,192 @@
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="D24" s="4">
-        <v>30305913000187</v>
+        <v>31462702000110</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25" s="2" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="D25" s="4">
-        <v>33882082000102</v>
+        <v>31462702000110</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="4">
-        <v>33882082000102</v>
+        <v>32110318000111</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I26" s="3">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="D27" s="4">
-        <v>31462702000110</v>
+        <v>32110318000111</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>96</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="I27" s="3">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D28" s="4">
-        <v>31462702000110</v>
+        <v>37575426000183</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I28" s="3">
-        <v>1</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="D29" s="4">
-        <v>32110318000111</v>
+        <v>37575426000183</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I29" s="3">
-        <v>1.5</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="4">
-        <v>32110318000111</v>
+        <v>97525817000115</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>96</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="I30" s="3">
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C31" s="2" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="D31" s="4">
-        <v>37575426000183</v>
+        <v>97525817000115</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C32" s="2" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="D32" s="4">
-        <v>37575426000183</v>
+        <v>34892058000109</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>97</v>
@@ -10686,163 +10607,155 @@
         <v>7</v>
       </c>
       <c r="D33" s="4">
-        <v>97525817000115</v>
+        <v>34892058000109</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I33" s="3">
-        <v>0.75</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" s="2" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="D34" s="4">
-        <v>97525817000115</v>
+        <v>13114958000155</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>96</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="I34" s="3">
-        <v>0.75</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" s="2" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="D35" s="4">
-        <v>34892058000109</v>
+        <v>13114958000155</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="3">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="D36" s="4">
-        <v>34892058000109</v>
+        <v>13114958000155</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I36" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" s="2" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="D37" s="4">
-        <v>13114958000155</v>
+        <v>12188730000147</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I37" s="3">
-        <v>4.5</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="2" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="D38" s="4">
-        <v>13114958000155</v>
+        <v>12188730000147</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I38" s="3">
-        <v>4.5</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C39" s="2" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="D39" s="4">
-        <v>13114958000155</v>
+        <v>18023366000141</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I39" s="3">
-        <v>1</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C40" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D40" s="4">
-        <v>12188730000147</v>
+        <v>18023366000141</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>8</v>
@@ -10858,13 +10771,13 @@
         <v>7</v>
       </c>
       <c r="D41" s="4">
-        <v>12188730000147</v>
+        <v>43953019000165</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>97</v>
@@ -10877,13 +10790,13 @@
         <v>7</v>
       </c>
       <c r="D42" s="4">
-        <v>18023366000141</v>
+        <v>43953019000165</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>97</v>
@@ -10893,16 +10806,16 @@
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C43" s="2" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="D43" s="4">
-        <v>18023366000141</v>
+        <v>44257405000185</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>97</v>
@@ -10912,16 +10825,16 @@
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C44" s="2" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="D44" s="4">
-        <v>43953019000165</v>
+        <v>44257405000185</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>97</v>
@@ -10931,51 +10844,59 @@
     </row>
     <row r="45" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C45" s="2" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="D45" s="4">
-        <v>43953019000165</v>
+        <v>24996797000197</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I45" s="3">
+        <v>1.95</v>
+      </c>
     </row>
     <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C46" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D46" s="4">
-        <v>44257405000185</v>
+        <v>24996797000197</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="3">
+        <v>1.95</v>
+      </c>
     </row>
     <row r="47" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C47" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D47" s="4">
-        <v>44257405000185</v>
+        <v>10992010000104</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>26</v>
@@ -10988,59 +10909,51 @@
     </row>
     <row r="48" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D48" s="4">
-        <v>24996797000197</v>
+        <v>10992010000104</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I48" s="3">
-        <v>1.95</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C49" s="2" t="s">
         <v>101</v>
       </c>
       <c r="D49" s="4">
-        <v>24996797000197</v>
+        <v>42111478000139</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I49" s="3">
-        <v>1.95</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C50" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D50" s="4">
-        <v>10992010000104</v>
+        <v>42111478000139</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>26</v>
@@ -11056,51 +10969,59 @@
         <v>95</v>
       </c>
       <c r="D51" s="4">
-        <v>10992010000104</v>
+        <v>28206152000164</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I51" s="3">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C52" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D52" s="4">
-        <v>42111478000139</v>
+        <v>28206152000164</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I52" s="3">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="53" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C53" s="2" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="D53" s="4">
-        <v>42111478000139</v>
+        <v>31156773000195</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>97</v>
@@ -11110,16 +11031,16 @@
     </row>
     <row r="54" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C54" s="2" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="D54" s="4">
-        <v>28206152000164</v>
+        <v>38099091000137</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>96</v>
@@ -11136,10 +11057,10 @@
         <v>95</v>
       </c>
       <c r="D55" s="4">
-        <v>28206152000164</v>
+        <v>22352091000167</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>26</v>
@@ -11148,97 +11069,32 @@
         <v>96</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="I55" s="3">
-        <v>1.5</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="56" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="D56" s="4">
-        <v>31156773000195</v>
+        <v>22352091000167</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-    </row>
-    <row r="57" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C57" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D57" s="4">
-        <v>38099091000137</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G57" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H57" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I57" s="3">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C58" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D58" s="4">
-        <v>22352091000167</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I58" s="3">
-        <v>1.95</v>
-      </c>
-    </row>
-    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C59" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D59" s="4">
-        <v>22352091000167</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H59" s="3" t="s">
+      <c r="H56" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I59" s="3">
+      <c r="I56" s="3">
         <v>1.95</v>
       </c>
     </row>
@@ -11252,37 +11108,37 @@
           <x14:formula1>
             <xm:f>Configurações!$H$3:$H$12</xm:f>
           </x14:formula1>
-          <xm:sqref>H9:H59</xm:sqref>
+          <xm:sqref>H6:H56</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ED7221E5-90E5-4E57-953C-2EBE44490DC4}">
           <x14:formula1>
             <xm:f>Configurações!$F$3:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G9:G59</xm:sqref>
+          <xm:sqref>G6:G56</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5DBF407A-E5B5-4ADB-A42B-762DE44E1343}">
           <x14:formula1>
             <xm:f>Configurações!$B$3:$B$71</xm:f>
           </x14:formula1>
-          <xm:sqref>F9:F59</xm:sqref>
+          <xm:sqref>F6:F56</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F3C01477-BD71-4418-BF61-26DC577C567E}">
           <x14:formula1>
             <xm:f>Configurações!$D$3:$D$14</xm:f>
           </x14:formula1>
-          <xm:sqref>E9:E14</xm:sqref>
+          <xm:sqref>E6:E11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A233C3B7-4BB9-4561-A5A2-008CD85E80B5}">
           <x14:formula1>
             <xm:f>Configurações!$D$3:$D$17</xm:f>
           </x14:formula1>
-          <xm:sqref>E15:E30</xm:sqref>
+          <xm:sqref>E12:E27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{743224EA-294A-4C3A-A14D-B17EBC59358E}">
           <x14:formula1>
             <xm:f>Configurações!$D$3:$D$20</xm:f>
           </x14:formula1>
-          <xm:sqref>E31:E59</xm:sqref>
+          <xm:sqref>E28:E56</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11295,7 +11151,7 @@
   <dimension ref="B2:J71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Alterações no scriptVync, add arquivo,atualizações
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filipe.nascimento\Desktop\vync\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EE177C-4CE4-4803-BDFB-A52CC824099D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE0AF4E-0811-436A-8DFF-33C3CBFE6202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{642F9480-EF3D-4509-A38C-60246068E5DF}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{642F9480-EF3D-4509-A38C-60246068E5DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
     <sheet name="Dezembro.2021" sheetId="3" r:id="rId2"/>
-    <sheet name="Configurações" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Configurações" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="115">
   <si>
     <t>nomeVendedor</t>
   </si>
@@ -352,6 +352,36 @@
   <si>
     <t>PICKUP 100_200</t>
   </si>
+  <si>
+    <t>05328923000190</t>
+  </si>
+  <si>
+    <t>CWB</t>
+  </si>
+  <si>
+    <t>PMW</t>
+  </si>
+  <si>
+    <t>BEL</t>
+  </si>
+  <si>
+    <t>BPS</t>
+  </si>
+  <si>
+    <t>SLZ</t>
+  </si>
+  <si>
+    <t>LGE</t>
+  </si>
+  <si>
+    <t>30036046000121</t>
+  </si>
+  <si>
+    <t>21545371009428</t>
+  </si>
+  <si>
+    <t>44324102000138</t>
+  </si>
 </sst>
 </file>
 
@@ -433,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -466,6 +496,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1179,7 +1215,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="4"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1188,7 +1224,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="B30" s="4"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1197,7 +1233,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" s="4"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1206,7 +1242,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="B32" s="4"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1215,7 +1251,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="4"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1224,7 +1260,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="4"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1233,7 +1269,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="4"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1242,7 +1278,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="B36" s="4"/>
+      <c r="B36" s="16"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1251,7 +1287,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="B37" s="4"/>
+      <c r="B37" s="16"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1260,7 +1296,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
-      <c r="B38" s="4"/>
+      <c r="B38" s="16"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1269,7 +1305,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
-      <c r="B39" s="4"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -9930,12 +9966,12 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F3C01477-BD71-4418-BF61-26DC577C567E}">
           <x14:formula1>
-            <xm:f>Configurações!$D$3:$D$20</xm:f>
+            <xm:f>Configurações!$D$3:$D$22</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1000</xm:sqref>
+          <xm:sqref>C40:C1000 C2:C3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5DBF407A-E5B5-4ADB-A42B-762DE44E1343}">
           <x14:formula1>
@@ -9955,6 +9991,12 @@
           </x14:formula1>
           <xm:sqref>F2:F1000</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F3183597-C7C3-4965-8DDF-4211DC81C2DC}">
+          <x14:formula1>
+            <xm:f>Configurações!$D$3:$D$21</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4:C39</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -9963,10 +10005,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EC228D-6414-49BA-B283-950DCE95B980}">
-  <dimension ref="A2:S56"/>
+  <dimension ref="A2:S149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="C150" sqref="C150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11098,29 +11140,1920 @@
         <v>1.95</v>
       </c>
     </row>
+    <row r="57" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D57" s="4">
+        <v>42090872000138</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I57" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C58" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D58" s="4">
+        <v>42090872000138</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I58" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C59" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D59" s="4">
+        <v>42090872000138</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I59" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C60" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D60" s="4">
+        <v>42090872000138</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I60" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C61" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D61" s="4">
+        <v>42090872000138</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I61" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C62" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D62" s="4">
+        <v>42090872000138</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I62" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C63" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D63" s="4">
+        <v>38447639000192</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I63" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C64" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D64" s="4">
+        <v>38447639000192</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I64" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C65" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D65" s="4">
+        <v>49021009000178</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I65" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="66" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C66" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="4">
+        <v>42871744000121</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I66" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="67" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C67" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D67" s="4">
+        <v>38356099000131</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I67" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C68" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D68" s="15">
+        <v>27445</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+    </row>
+    <row r="69" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C69" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="4">
+        <v>33646642000111</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+    </row>
+    <row r="70" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C70" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="4">
+        <v>33646642000111</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+    </row>
+    <row r="71" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C71" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="4">
+        <v>32734547000107</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+    </row>
+    <row r="72" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C72" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="4">
+        <v>32734547000107</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+    </row>
+    <row r="73" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C73" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="4">
+        <v>33990460000163</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+    </row>
+    <row r="74" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C74" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="4">
+        <v>33990460000163</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+    </row>
+    <row r="75" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C75" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D75" s="4">
+        <v>42417100000168</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I75" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="76" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C76" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="4">
+        <v>40797625000140</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+    </row>
+    <row r="77" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C77" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="4">
+        <v>40797625000140</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+    </row>
+    <row r="78" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C78" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" s="4">
+        <v>2175591000163</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+    </row>
+    <row r="79" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C79" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" s="4">
+        <v>2175591000163</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+    </row>
+    <row r="80" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C80" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D80" s="4">
+        <v>18404704000195</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+    </row>
+    <row r="81" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C81" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D81" s="4">
+        <v>18404704000195</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
+    </row>
+    <row r="82" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C82" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I82" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="83" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C83" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I83" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="84" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C84" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D84" s="4">
+        <v>38200020000189</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H84" s="3"/>
+      <c r="I84" s="3"/>
+    </row>
+    <row r="85" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C85" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D85" s="4">
+        <v>38200020000189</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H85" s="3"/>
+      <c r="I85" s="3"/>
+    </row>
+    <row r="86" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C86" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D86" s="4">
+        <v>38200020000189</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H86" s="3"/>
+      <c r="I86" s="3"/>
+    </row>
+    <row r="87" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C87" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" s="4">
+        <v>29590641000125</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H87" s="3"/>
+      <c r="I87" s="3"/>
+    </row>
+    <row r="88" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C88" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88" s="4">
+        <v>29590641000125</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H88" s="3"/>
+      <c r="I88" s="3"/>
+    </row>
+    <row r="89" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C89" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89" s="4">
+        <v>12863194000138</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I89" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="90" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C90" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90" s="4">
+        <v>12863194000138</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I90" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="91" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C91" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D91" s="4">
+        <v>38450737000189</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I91" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="92" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C92" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D92" s="4">
+        <v>38450737000189</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I92" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="93" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C93" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D93" s="4">
+        <v>38450737000189</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I93" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C94" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D94" s="4">
+        <v>38450737000189</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I94" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C95" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D95" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H95" s="3"/>
+      <c r="I95" s="3"/>
+    </row>
+    <row r="96" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C96" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D96" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H96" s="3"/>
+      <c r="I96" s="3"/>
+    </row>
+    <row r="97" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C97" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D97" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H97" s="3"/>
+      <c r="I97" s="3"/>
+    </row>
+    <row r="98" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C98" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D98" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H98" s="3"/>
+      <c r="I98" s="3"/>
+    </row>
+    <row r="99" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C99" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D99" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H99" s="3"/>
+      <c r="I99" s="3"/>
+    </row>
+    <row r="100" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C100" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D100" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H100" s="3"/>
+      <c r="I100" s="3"/>
+    </row>
+    <row r="101" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C101" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D101" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H101" s="3"/>
+      <c r="I101" s="3"/>
+    </row>
+    <row r="102" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C102" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D102" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H102" s="3"/>
+      <c r="I102" s="3"/>
+    </row>
+    <row r="103" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C103" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D103" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H103" s="3"/>
+      <c r="I103" s="3"/>
+    </row>
+    <row r="104" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C104" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D104" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H104" s="3"/>
+      <c r="I104" s="3"/>
+    </row>
+    <row r="105" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C105" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D105" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H105" s="3"/>
+      <c r="I105" s="3"/>
+    </row>
+    <row r="106" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C106" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D106" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H106" s="3"/>
+      <c r="I106" s="3"/>
+    </row>
+    <row r="107" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C107" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D107" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H107" s="3"/>
+      <c r="I107" s="3"/>
+    </row>
+    <row r="108" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C108" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D108" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H108" s="3"/>
+      <c r="I108" s="3"/>
+    </row>
+    <row r="109" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C109" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H109" s="3"/>
+      <c r="I109" s="3"/>
+    </row>
+    <row r="110" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C110" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D110" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H110" s="3"/>
+      <c r="I110" s="3"/>
+    </row>
+    <row r="111" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C111" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D111" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H111" s="3"/>
+      <c r="I111" s="3"/>
+    </row>
+    <row r="112" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C112" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D112" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H112" s="3"/>
+      <c r="I112" s="3"/>
+    </row>
+    <row r="113" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C113" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D113" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H113" s="3"/>
+      <c r="I113" s="3"/>
+    </row>
+    <row r="114" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C114" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D114" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H114" s="3"/>
+      <c r="I114" s="3"/>
+    </row>
+    <row r="115" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C115" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D115" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H115" s="3"/>
+      <c r="I115" s="3"/>
+    </row>
+    <row r="116" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C116" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D116" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H116" s="3"/>
+      <c r="I116" s="3"/>
+    </row>
+    <row r="117" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C117" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D117" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H117" s="3"/>
+      <c r="I117" s="3"/>
+    </row>
+    <row r="118" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C118" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D118" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H118" s="3"/>
+      <c r="I118" s="3"/>
+    </row>
+    <row r="119" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C119" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D119" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H119" s="3"/>
+      <c r="I119" s="3"/>
+    </row>
+    <row r="120" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C120" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D120" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H120" s="3"/>
+      <c r="I120" s="3"/>
+    </row>
+    <row r="121" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C121" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D121" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H121" s="3"/>
+      <c r="I121" s="3"/>
+    </row>
+    <row r="122" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C122" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D122" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G122" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H122" s="3"/>
+      <c r="I122" s="3"/>
+    </row>
+    <row r="123" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C123" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D123" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H123" s="3"/>
+      <c r="I123" s="3"/>
+    </row>
+    <row r="124" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C124" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D124" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H124" s="3"/>
+      <c r="I124" s="3"/>
+    </row>
+    <row r="125" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C125" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D125" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H125" s="3"/>
+      <c r="I125" s="3"/>
+    </row>
+    <row r="126" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C126" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D126" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G126" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H126" s="3"/>
+      <c r="I126" s="3"/>
+    </row>
+    <row r="127" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C127" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D127" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G127" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H127" s="3"/>
+      <c r="I127" s="3"/>
+    </row>
+    <row r="128" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C128" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D128" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H128" s="3"/>
+      <c r="I128" s="3"/>
+    </row>
+    <row r="129" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C129" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D129" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G129" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H129" s="3"/>
+      <c r="I129" s="3"/>
+    </row>
+    <row r="130" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C130" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D130" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G130" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H130" s="3"/>
+      <c r="I130" s="3"/>
+    </row>
+    <row r="131" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C131" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D131" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H131" s="3"/>
+      <c r="I131" s="3"/>
+    </row>
+    <row r="132" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C132" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D132" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G132" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H132" s="3"/>
+      <c r="I132" s="3"/>
+    </row>
+    <row r="133" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C133" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D133" s="4">
+        <v>33075215000120</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G133" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H133" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I133" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="134" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C134" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D134" s="4">
+        <v>33075215000120</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G134" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H134" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I134" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="135" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C135" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D135" s="4">
+        <v>35463878000148</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G135" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H135" s="3"/>
+      <c r="I135" s="3"/>
+    </row>
+    <row r="136" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C136" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D136" s="4">
+        <v>35463878000148</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G136" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H136" s="3"/>
+      <c r="I136" s="3"/>
+    </row>
+    <row r="137" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C137" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D137" s="4">
+        <v>37826074000191</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G137" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H137" s="3"/>
+      <c r="I137" s="3"/>
+    </row>
+    <row r="138" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C138" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D138" s="4">
+        <v>37826074000191</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G138" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H138" s="3"/>
+      <c r="I138" s="3"/>
+    </row>
+    <row r="139" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C139" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D139" s="4">
+        <v>29590641000125</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G139" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H139" s="3"/>
+      <c r="I139" s="3"/>
+    </row>
+    <row r="140" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C140" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D140" s="4">
+        <v>29590641000125</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H140" s="3"/>
+      <c r="I140" s="3"/>
+    </row>
+    <row r="141" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C141" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D141" s="4">
+        <v>36696851000168</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G141" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H141" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I141" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="142" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C142" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D142" s="4">
+        <v>36696851000168</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I142" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="143" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C143" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D143" s="4">
+        <v>36696851000168</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G143" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H143" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I143" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="144" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C144" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D144" s="4">
+        <v>41100476000181</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G144" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H144" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I144" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="145" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C145" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D145" s="4">
+        <v>41100476000181</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G145" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H145" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I145" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="146" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C146" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D146" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G146" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H146" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I146" s="3">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="147" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C147" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D147" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G147" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H147" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I147" s="3">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="148" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C148" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D148" s="4">
+        <v>42236293000150</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G148" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H148" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I148" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C149" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D149" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G149" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H149" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I149" s="3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0F8627C6-C092-4293-9362-50A35151177D}">
           <x14:formula1>
             <xm:f>Configurações!$H$3:$H$12</xm:f>
           </x14:formula1>
-          <xm:sqref>H6:H56</xm:sqref>
+          <xm:sqref>H6:H149</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ED7221E5-90E5-4E57-953C-2EBE44490DC4}">
           <x14:formula1>
             <xm:f>Configurações!$F$3:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G6:G56</xm:sqref>
+          <xm:sqref>G6:G149</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5DBF407A-E5B5-4ADB-A42B-762DE44E1343}">
           <x14:formula1>
             <xm:f>Configurações!$B$3:$B$71</xm:f>
           </x14:formula1>
-          <xm:sqref>F6:F56</xm:sqref>
+          <xm:sqref>F6:F149</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F3C01477-BD71-4418-BF61-26DC577C567E}">
           <x14:formula1>
@@ -11140,6 +13073,18 @@
           </x14:formula1>
           <xm:sqref>E28:E56</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C95E7846-C9C2-41C7-B292-475929F31C87}">
+          <x14:formula1>
+            <xm:f>Configurações!$D$3:$D$21</xm:f>
+          </x14:formula1>
+          <xm:sqref>E57:E83 E95:E132 E146:E147</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{892F224A-83CD-4D22-BEAC-4948AA737896}">
+          <x14:formula1>
+            <xm:f>Configurações!$D$3:$D$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>E84:E94 E133:E145 E148:E149</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -11151,7 +13096,7 @@
   <dimension ref="B2:J71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11335,7 +13280,7 @@
         <v>35</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>103</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
@@ -11343,15 +13288,15 @@
         <v>36</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>88</v>
+      <c r="D16" s="14" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -11359,7 +13304,7 @@
         <v>38</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -11367,7 +13312,7 @@
         <v>39</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -11375,7 +13320,7 @@
         <v>40</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -11383,17 +13328,23 @@
         <v>28</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>41</v>
       </c>
+      <c r="D21" s="7" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>42</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Novos registros de email.
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filipe.nascimento\Desktop\vync\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FD64EC-7CA5-47A0-9F9B-631E58FA7C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44953F5B-0207-44FE-B0E1-8307A367924F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{642F9480-EF3D-4509-A38C-60246068E5DF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="115">
   <si>
     <t>nomeVendedor</t>
   </si>
@@ -933,7 +933,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10005,10 +10005,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EC228D-6414-49BA-B283-950DCE95B980}">
-  <dimension ref="A2:S149"/>
+  <dimension ref="A2:S152"/>
   <sheetViews>
     <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="C150" sqref="C150"/>
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13031,23 +13031,92 @@
         <v>1</v>
       </c>
     </row>
+    <row r="150" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C150" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D150" s="4">
+        <v>37685370000110</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G150" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H150" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I150" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="151" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C151" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D151" s="4">
+        <v>37685370000110</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G151" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H151" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I151" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="152" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C152" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D152" s="4">
+        <v>37685370000110</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F152" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G152" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H152" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I152" s="3">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0F8627C6-C092-4293-9362-50A35151177D}">
           <x14:formula1>
             <xm:f>Configurações!$H$3:$H$12</xm:f>
           </x14:formula1>
-          <xm:sqref>H6:H149</xm:sqref>
+          <xm:sqref>H6:H152</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ED7221E5-90E5-4E57-953C-2EBE44490DC4}">
           <x14:formula1>
             <xm:f>Configurações!$F$3:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G6:G149</xm:sqref>
+          <xm:sqref>G6:G152</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5DBF407A-E5B5-4ADB-A42B-762DE44E1343}">
           <x14:formula1>
@@ -13083,7 +13152,13 @@
           <x14:formula1>
             <xm:f>Configurações!$D$3:$D$22</xm:f>
           </x14:formula1>
-          <xm:sqref>E84:E94 E133:E145 E148:E149</xm:sqref>
+          <xm:sqref>E84:E94 E133:E145 E148:E152</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F04D8621-3333-457C-8C2E-9CE0FE05A120}">
+          <x14:formula1>
+            <xm:f>Configurações!$B$3:$B$72</xm:f>
+          </x14:formula1>
+          <xm:sqref>F150:F152</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Novos Scripts de Emails Gerados.
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filipe.nascimento\Desktop\vync\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44953F5B-0207-44FE-B0E1-8307A367924F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E4BEA5-8798-44AD-9E18-0173E7A62682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{642F9480-EF3D-4509-A38C-60246068E5DF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="115">
   <si>
     <t>nomeVendedor</t>
   </si>
@@ -10005,10 +10005,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EC228D-6414-49BA-B283-950DCE95B980}">
-  <dimension ref="A2:S152"/>
+  <dimension ref="A2:S155"/>
   <sheetViews>
     <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="C153" sqref="C153"/>
+      <selection activeCell="C156" sqref="C156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13100,6 +13100,67 @@
         <v>10</v>
       </c>
     </row>
+    <row r="153" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C153" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D153" s="4">
+        <v>41543621000107</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G153" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H153" s="3"/>
+      <c r="I153" s="3"/>
+    </row>
+    <row r="154" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C154" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D154" s="4">
+        <v>41543621000107</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G154" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H154" s="3"/>
+      <c r="I154" s="3"/>
+    </row>
+    <row r="155" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C155" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D155" s="4">
+        <v>32391894000184</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F155" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G155" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H155" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I155" s="3">
+        <v>2.95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -13110,13 +13171,13 @@
           <x14:formula1>
             <xm:f>Configurações!$H$3:$H$12</xm:f>
           </x14:formula1>
-          <xm:sqref>H6:H152</xm:sqref>
+          <xm:sqref>H6:H155</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ED7221E5-90E5-4E57-953C-2EBE44490DC4}">
           <x14:formula1>
             <xm:f>Configurações!$F$3:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G6:G152</xm:sqref>
+          <xm:sqref>G6:G155</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5DBF407A-E5B5-4ADB-A42B-762DE44E1343}">
           <x14:formula1>
@@ -13152,13 +13213,13 @@
           <x14:formula1>
             <xm:f>Configurações!$D$3:$D$22</xm:f>
           </x14:formula1>
-          <xm:sqref>E84:E94 E133:E145 E148:E152</xm:sqref>
+          <xm:sqref>E84:E94 E133:E145 E148:E155</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F04D8621-3333-457C-8C2E-9CE0FE05A120}">
           <x14:formula1>
             <xm:f>Configurações!$B$3:$B$72</xm:f>
           </x14:formula1>
-          <xm:sqref>F150:F152</xm:sqref>
+          <xm:sqref>F150:F155</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>